<commit_message>
updating utilities and screenshot
</commit_message>
<xml_diff>
--- a/TestWorkbook.xlsx
+++ b/TestWorkbook.xlsx
@@ -4,22 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="12885" windowHeight="5550"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="12885" windowHeight="3765" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="departingData" sheetId="4" r:id="rId4"/>
+    <sheet name="Searchflightdata" sheetId="4" r:id="rId4"/>
     <sheet name="arrivingData" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:M17"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>mercury</t>
   </si>
@@ -49,6 +48,27 @@
   </si>
   <si>
     <t>ongoing</t>
+  </si>
+  <si>
+    <t>city1</t>
+  </si>
+  <si>
+    <t>city2</t>
+  </si>
+  <si>
+    <t>city3</t>
+  </si>
+  <si>
+    <t>city4</t>
+  </si>
+  <si>
+    <t>city5</t>
+  </si>
+  <si>
+    <t>fromcity</t>
+  </si>
+  <si>
+    <t>tocity</t>
   </si>
 </sst>
 </file>
@@ -396,7 +416,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -489,38 +509,38 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -530,37 +550,52 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>